<commit_message>
remove old values for foodsecurity
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2016Aug02/validation/Input_Bangladesh_2016_1604_LiST.xlsx
+++ b/input_spreadsheets/Bangladesh/2016Aug02/validation/Input_Bangladesh_2016_1604_LiST.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-4920" yWindow="-21040" windowWidth="32160" windowHeight="19240" tabRatio="500" firstSheet="14" activeTab="21"/>
+    <workbookView xWindow="-4920" yWindow="-21040" windowWidth="32160" windowHeight="19240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -417,9 +417,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -497,7 +498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -544,6 +545,7 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -611,6 +613,159 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -632,6 +787,159 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2049" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 1" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -933,10 +1241,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -944,7 +1252,7 @@
     <col min="1" max="1" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -952,7 +1260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -960,7 +1268,7 @@
         <v>14790000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -968,7 +1276,7 @@
         <v>3030000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -976,32 +1284,41 @@
         <v>3583822</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="2">
-        <v>0.56999999999999995</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B6" s="21">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>0.4365</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B7" s="21">
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="22"/>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C11" s="21"/>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C12" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2398,7 +2715,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>63</v>
       </c>
@@ -2467,7 +2784,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>42</v>
       </c>
@@ -3013,11 +3330,11 @@
       </c>
       <c r="D5" s="23">
         <f>demographics!$B$6</f>
-        <v>0.4</v>
+        <v>0.4365</v>
       </c>
       <c r="E5" s="23">
         <f>demographics!$B$6</f>
-        <v>0.4</v>
+        <v>0.4365</v>
       </c>
       <c r="F5" s="5">
         <v>0</v>
@@ -3070,7 +3387,7 @@
       </c>
       <c r="G7" s="23">
         <f>demographics!$B$6</f>
-        <v>0.4</v>
+        <v>0.4365</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3202,7 +3519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -3257,11 +3574,11 @@
       </c>
       <c r="C3" s="18">
         <f>demographics!$B$5 * 'Interventions target population'!$G$7</f>
-        <v>0.22799999999999998</v>
+        <v>0.4365</v>
       </c>
       <c r="D3" s="18">
         <f>demographics!$B$5 * 'Interventions target population'!$G$7</f>
-        <v>0.22799999999999998</v>
+        <v>0.4365</v>
       </c>
       <c r="E3" s="18">
         <v>0</v>
@@ -3772,7 +4089,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>23.3</v>
       </c>

</xml_diff>